<commit_message>
setup RESET signal to GND, active HIGH
</commit_message>
<xml_diff>
--- a/layout/busanalizer/Project Outputs for BusAnalizer/BOM/Bill of Materials-busanalizer.xlsx
+++ b/layout/busanalizer/Project Outputs for BusAnalizer/BOM/Bill of Materials-busanalizer.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECF0BC9F-6199-4579-9ABD-DA0D5AB594F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC58B094-0C64-4222-B23A-6CA3BE09807C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{44D1F457-A872-47FA-AF89-A35903121825}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{E5DDBD57-E5FA-43C8-93B1-2DC5208969FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-busanalizer" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
     <t>&lt;B&gt;RESISTOR&lt;/B&gt;, European symbol, [NoValue]</t>
   </si>
   <si>
-    <t>R2, R4, R5, R6, R7, R8, R10, R11, R12, R13, R15, R24</t>
+    <t>R2, R4, R5, R6, R7, R8, R10, R11, R12, R13, R15, R24, R50</t>
   </si>
   <si>
     <t>1M</t>
@@ -781,7 +781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9CDC-45E3-4E79-A78C-61FED14BD9C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5808981-901F-4A5E-AD07-14703406869A}">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1328,7 +1328,7 @@
         <v>85</v>
       </c>
       <c r="F27" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
generate the fabrication files
</commit_message>
<xml_diff>
--- a/layout/busanalizer/Project Outputs for BusAnalizer/BOM/Bill of Materials-busanalizer.xlsx
+++ b/layout/busanalizer/Project Outputs for BusAnalizer/BOM/Bill of Materials-busanalizer.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC58B094-0C64-4222-B23A-6CA3BE09807C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{461CE5B7-4A1F-43C0-B085-05158D1852AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{E5DDBD57-E5FA-43C8-93B1-2DC5208969FA}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{D3CD79BF-068F-4A15-8AD6-8BEC4F825634}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-busanalizer" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="127">
   <si>
     <t>Comment</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t>SV1</t>
+  </si>
+  <si>
+    <t>TPB2,54</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Test pad&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>TP2</t>
+  </si>
+  <si>
+    <t>B2,54</t>
   </si>
   <si>
     <t>KF33D</t>
@@ -781,8 +793,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5808981-901F-4A5E-AD07-14703406869A}">
-  <dimension ref="A1:F39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15298A3-09D1-4C49-95C2-B43221778D69}">
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1496,13 +1508,13 @@
         <v>110</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>110</v>
@@ -1513,49 +1525,49 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="F37" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="F38" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="64.5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -1568,6 +1580,26 @@
         <v>119</v>
       </c>
       <c r="F39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rework after pcb manufacterer remarks
</commit_message>
<xml_diff>
--- a/layout/busanalizer/Project Outputs for BusAnalizer/BOM/Bill of Materials-busanalizer.xlsx
+++ b/layout/busanalizer/Project Outputs for BusAnalizer/BOM/Bill of Materials-busanalizer.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA62BE97-66A2-4EF4-BAC5-9B656B482D6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4D471BF-C166-484C-96BB-CD362A189F97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{4AC3682E-C23F-4108-8FF0-DC8F98895C19}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{15846CDF-741F-4479-A2A9-4024727DB847}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-busanalizer" sheetId="1" r:id="rId1"/>
@@ -793,7 +793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9362E3C6-B995-43BF-A604-F28F6D806583}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725EEC90-5828-4774-8078-A76FAC9D1273}">
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>